<commit_message>
Refactored code and fixed parser.
</commit_message>
<xml_diff>
--- a/upload/test1.xlsx
+++ b/upload/test1.xlsx
@@ -376,7 +376,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,9 +469,6 @@
       <c r="B8">
         <v>5</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>